<commit_message>
Updated schedule and requirements document based on technology committee meeting of 7/12/2023.
</commit_message>
<xml_diff>
--- a/ProjectSchedule.xlsx
+++ b/ProjectSchedule.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulC\Documents\PersonalMacWin\BHHS_Reunion\DevelDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulC\Documents\ProjectsNfwsi\BHHS_74_50th_Reunion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E241EA-03E5-4258-9784-25BD29849636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E574AD2-81EC-4EDE-8859-C76E62012324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Task Number</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Task 1</t>
-  </si>
-  <si>
-    <t>Tasks 1 &amp; 2</t>
   </si>
   <si>
     <t>Set up basic theme (black, white orange)</t>
@@ -71,12 +68,6 @@
   <si>
     <t>Put holding web page in place
 Welcome to the BHHS Class of 1974 50th Reunion Website</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
   </si>
   <si>
     <t>Set up committee pages</t>
@@ -123,13 +114,65 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>In Process</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
     <t>Set up ecommerce portion of website for purchasing tickets</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Buy Divi Theme from Elegant Themes</t>
+  </si>
+  <si>
+    <t>Events Committee</t>
+  </si>
+  <si>
+    <t>Select Venue
+Select Date</t>
+  </si>
+  <si>
+    <t>8 weeks</t>
+  </si>
+  <si>
+    <t>6 Hrs</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Ruth Amir</t>
+  </si>
+  <si>
+    <t>1 Week</t>
+  </si>
+  <si>
+    <t>Graphic Design for website</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Graphic Design to website </t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>Final Graphic Design with Ad Copy</t>
+  </si>
+  <si>
+    <t>Elementary School Reunion web pages</t>
   </si>
 </sst>
 </file>
@@ -487,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -543,15 +586,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="7">
         <v>45118</v>
@@ -560,10 +603,10 @@
         <v>45119</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>9</v>
@@ -576,56 +619,68 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="7">
         <v>45485</v>
       </c>
+      <c r="E4" s="7">
+        <v>45119</v>
+      </c>
       <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7">
+        <v>45119</v>
+      </c>
+      <c r="E5" s="7">
+        <v>45120</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7">
+        <v>45119</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -633,17 +688,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,12 +706,15 @@
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -666,154 +722,277 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="7">
-        <v>45292</v>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D13" s="7">
-        <v>45138</v>
+        <v>45124</v>
+      </c>
+      <c r="E13" s="7">
+        <v>45170</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7">
-        <v>45230</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
       <c r="G15" s="3"/>
       <c r="H15" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="7">
+        <v>45292</v>
+      </c>
+      <c r="E16" s="7">
+        <v>44985</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="7">
+        <v>45138</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="7">
+        <v>45230</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G19" s="3"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G20" s="3"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G21" s="3"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G22" s="3"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G23" s="3"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" s="3"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G25" s="3"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G26" s="3"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G27" s="3"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G28" s="3"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" s="3"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32" s="3"/>
       <c r="H32" s="6"/>
     </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="3"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="3"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="3"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="3"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="3"/>
+      <c r="H38" s="6"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H21">
+    <sortCondition ref="A3:A21"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>

</xml_diff>